<commit_message>
completing old work #1
</commit_message>
<xml_diff>
--- a/Admin_&_References/Attendance_Record.xlsx
+++ b/Admin_&_References/Attendance_Record.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,15 +554,52 @@
       <c r="C11" s="1" t="str">
         <v>06-02-2026</v>
       </c>
+      <c r="D11" s="1" t="str">
+        <v>yes</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
         <v>11</v>
       </c>
+      <c r="B12" s="1" t="str">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>07-02-2026</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="str">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v>null</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v>08-02-2026</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v>sunday</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="str">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v>09-02-2026</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
day 18 on hold
</commit_message>
<xml_diff>
--- a/Admin_&_References/Attendance_Record.xlsx
+++ b/Admin_&_References/Attendance_Record.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -708,10 +708,35 @@
       <c r="C22" s="1" t="str">
         <v>17-02-2026</v>
       </c>
+      <c r="D22" s="1" t="str">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <v>18-02-2026</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <v>19-02-2026</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
readme updated and day 20
</commit_message>
<xml_diff>
--- a/Admin_&_References/Attendance_Record.xlsx
+++ b/Admin_&_References/Attendance_Record.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -744,10 +744,85 @@
       <c r="A25" s="1" t="str">
         <v>24</v>
       </c>
+      <c r="B25" s="1" t="str">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <v>20-02-20206</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="str">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <v>21-02-2026</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="str">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <v>null</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <v>22-02-2026</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <v>sunday</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="str">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <v>23</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <v>23-02-2026</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="str">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>24-02-2026</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="str">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>25-02-2026</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="str">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <v>26</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <v>26-02-2026</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>